<commit_message>
begin data passthrough circuitry
</commit_message>
<xml_diff>
--- a/CPU.xlsx
+++ b/CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\Microcontroller\CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F05D29-7896-4595-AC06-B59AA98FE1C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9344BCA8-1BAB-45CD-8B48-F619996AB4AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="599" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstructionSet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="492">
   <si>
     <t>Instruction Format</t>
   </si>
@@ -1494,6 +1494,24 @@
   <si>
     <t>// PC++</t>
   </si>
+  <si>
+    <t>Move Data</t>
+  </si>
+  <si>
+    <t>Source In</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
 </sst>
 </file>
 
@@ -1562,10 +1580,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1901,29 +1919,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP214"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9:AO9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
     <col min="12" max="12" width="5" customWidth="1"/>
     <col min="13" max="13" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
     <col min="16" max="16" width="8.42578125" customWidth="1"/>
-    <col min="17" max="17" width="4" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
     <col min="19" max="19" width="17.28515625" customWidth="1"/>
     <col min="20" max="20" width="5.42578125" customWidth="1"/>
@@ -1945,27 +1963,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
@@ -1983,30 +2001,30 @@
       </c>
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="H2" s="9"/>
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="K2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="P2" s="8" t="s">
+      <c r="N2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="9"/>
       <c r="S2" t="s">
         <v>11</v>
       </c>
@@ -2163,51 +2181,51 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
-      <c r="AC3" s="9" t="s">
+      <c r="AC3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9" t="s">
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9" t="s">
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9" t="s">
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
       <c r="AM3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="9" t="s">
+      <c r="AN3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AO3" s="9"/>
+      <c r="AO3" s="8"/>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
-      <c r="AS3" s="9" t="s">
+      <c r="AS3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AT3" s="9"/>
-      <c r="AU3" s="9"/>
-      <c r="AV3" s="9"/>
-      <c r="AW3" s="9"/>
-      <c r="AX3" s="9"/>
-      <c r="AY3" s="9"/>
-      <c r="AZ3" s="9"/>
-      <c r="BA3" s="9"/>
-      <c r="BB3" s="9"/>
-      <c r="BC3" s="9"/>
-      <c r="BD3" s="9"/>
-      <c r="BE3" s="9"/>
-      <c r="BF3" s="9"/>
-      <c r="BG3" s="9"/>
-      <c r="BH3" s="9"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8"/>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="8"/>
+      <c r="BH3" s="8"/>
     </row>
     <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="AC4" s="1"/>
@@ -3390,9 +3408,18 @@
       </c>
     </row>
     <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>486</v>
+      </c>
+      <c r="B11" s="1">
+        <v>110</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
+      <c r="J11" t="s">
+        <v>490</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>80</v>
       </c>
@@ -3794,6 +3821,9 @@
       </c>
     </row>
     <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>489</v>
+      </c>
       <c r="U13" t="s">
         <v>460</v>
       </c>
@@ -3978,6 +4008,9 @@
       </c>
     </row>
     <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>487</v>
+      </c>
       <c r="U14" t="s">
         <v>461</v>
       </c>
@@ -4162,6 +4195,9 @@
       </c>
     </row>
     <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="U15" t="s">
         <v>462</v>
       </c>
@@ -4530,6 +4566,12 @@
       </c>
     </row>
     <row r="17" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="U17" t="s">
         <v>464</v>
       </c>
@@ -4714,6 +4756,10 @@
       </c>
     </row>
     <row r="18" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="J18" s="2"/>
       <c r="U18" t="s">
         <v>465</v>
@@ -4902,7 +4948,9 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -5108,7 +5156,9 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -5314,6 +5364,10 @@
       </c>
     </row>
     <row r="21" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="1"/>
       <c r="U21" t="s">
         <v>468</v>
       </c>
@@ -5507,6 +5561,10 @@
       </c>
     </row>
     <row r="22" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="U22" t="s">
         <v>469</v>
       </c>
@@ -5700,6 +5758,10 @@
       </c>
     </row>
     <row r="23" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="U23" t="s">
         <v>62</v>
       </c>
@@ -5887,6 +5949,10 @@
       </c>
     </row>
     <row r="24" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>490</v>
+      </c>
+      <c r="E24" s="1"/>
       <c r="U24" t="s">
         <v>70</v>
       </c>
@@ -6071,6 +6137,9 @@
       </c>
     </row>
     <row r="25" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>491</v>
+      </c>
       <c r="U25" t="s">
         <v>74</v>
       </c>
@@ -6255,6 +6324,9 @@
       </c>
     </row>
     <row r="26" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>378</v>
+      </c>
       <c r="U26" t="s">
         <v>78</v>
       </c>
@@ -6439,6 +6511,9 @@
       </c>
     </row>
     <row r="27" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
       <c r="U27" t="s">
         <v>81</v>
       </c>
@@ -38842,12 +38917,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AS3:BH3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
@@ -38855,6 +38924,12 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AS3:BH3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AN3:AO3"/>
   </mergeCells>
   <conditionalFormatting sqref="AC42:BG47">
     <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
@@ -40066,8 +40141,8 @@
   </sheetPr>
   <dimension ref="A1:CL110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BF4" sqref="BF4:BF70"/>
+    <sheetView topLeftCell="Q39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX60" sqref="U60:AX60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40107,27 +40182,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:90" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
       <c r="T1" t="s">
         <v>370</v>
       </c>
@@ -40145,30 +40220,30 @@
       </c>
     </row>
     <row r="2" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="H2" s="9"/>
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="K2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="P2" s="8" t="s">
+      <c r="N2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="9"/>
       <c r="S2" t="s">
         <v>11</v>
       </c>
@@ -40322,60 +40397,60 @@
       <c r="S3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8" t="s">
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8" t="s">
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
       <c r="AL3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AM3" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8" t="s">
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8" t="s">
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8" t="s">
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="9"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8" t="s">
+      <c r="AV3" s="9"/>
+      <c r="AW3" s="9"/>
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8" t="s">
+      <c r="AZ3" s="9"/>
+      <c r="BA3" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="8" t="s">
+      <c r="BB3" s="9"/>
+      <c r="BC3" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="BD3" s="8"/>
+      <c r="BD3" s="9"/>
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.25">
       <c r="Y4">
@@ -52790,11 +52865,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="AU3:AX3"/>
-    <mergeCell ref="AQ3:AT3"/>
-    <mergeCell ref="AM3:AN3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="AO3:AP3"/>
     <mergeCell ref="A1:S1"/>
@@ -52807,6 +52877,11 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="AU3:AX3"/>
+    <mergeCell ref="AQ3:AT3"/>
+    <mergeCell ref="AM3:AN3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
begin instruction set V2
</commit_message>
<xml_diff>
--- a/CPU.xlsx
+++ b/CPU.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\Microcontroller\CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\GitHub\CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9344BCA8-1BAB-45CD-8B48-F619996AB4AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C11F2-A3F0-4AB8-A555-DFDBE0DE17C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstructionSet" sheetId="1" r:id="rId1"/>
-    <sheet name="Set" sheetId="5" r:id="rId2"/>
-    <sheet name="FetchExecuteCycle" sheetId="2" r:id="rId3"/>
+    <sheet name="InstructioneSetV2" sheetId="6" r:id="rId2"/>
+    <sheet name="Set" sheetId="5" r:id="rId3"/>
+    <sheet name="FetchExecuteCycle" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="507">
   <si>
     <t>Instruction Format</t>
   </si>
@@ -1512,12 +1513,57 @@
   <si>
     <t>CR</t>
   </si>
+  <si>
+    <t>RV</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>DivMod</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>RRV</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SHR</t>
+  </si>
+  <si>
+    <t>SHL</t>
+  </si>
+  <si>
+    <t>SHLR</t>
+  </si>
+  <si>
+    <t>SHLL</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>NEG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1546,13 +1592,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1564,10 +1622,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1580,14 +1639,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -1919,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP214"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1963,27 +2024,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
@@ -2001,30 +2062,30 @@
       </c>
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="K2" s="8"/>
+      <c r="M2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="P2" s="9" t="s">
+      <c r="N2" s="8"/>
+      <c r="P2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="8"/>
       <c r="S2" t="s">
         <v>11</v>
       </c>
@@ -2181,51 +2242,51 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
-      <c r="AC3" s="8" t="s">
+      <c r="AC3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8" t="s">
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8" t="s">
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8" t="s">
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
       <c r="AM3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AN3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AO3" s="8"/>
+      <c r="AO3" s="9"/>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
-      <c r="AS3" s="8" t="s">
+      <c r="AS3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8"/>
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="8"/>
-      <c r="BD3" s="8"/>
-      <c r="BE3" s="8"/>
-      <c r="BF3" s="8"/>
-      <c r="BG3" s="8"/>
-      <c r="BH3" s="8"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9"/>
+      <c r="AV3" s="9"/>
+      <c r="AW3" s="9"/>
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="9"/>
+      <c r="AZ3" s="9"/>
+      <c r="BA3" s="9"/>
+      <c r="BB3" s="9"/>
+      <c r="BC3" s="9"/>
+      <c r="BD3" s="9"/>
+      <c r="BE3" s="9"/>
+      <c r="BF3" s="9"/>
+      <c r="BG3" s="9"/>
+      <c r="BH3" s="9"/>
     </row>
     <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="AC4" s="1"/>
@@ -38917,6 +38978,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AS3:BH3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
@@ -38924,12 +38991,6 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AS3:BH3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AN3:AO3"/>
   </mergeCells>
   <conditionalFormatting sqref="AC42:BG47">
     <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
@@ -38976,6 +39037,472 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F503B65-843C-459C-96CC-4F6A4CE4A550}">
+  <dimension ref="A2:B60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>494</v>
+      </c>
+      <c r="B9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B10" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>495</v>
+      </c>
+      <c r="B11" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>495</v>
+      </c>
+      <c r="B12" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>496</v>
+      </c>
+      <c r="B19" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>497</v>
+      </c>
+      <c r="B21" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>499</v>
+      </c>
+      <c r="B22" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>365</v>
+      </c>
+      <c r="B24" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>367</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>367</v>
+      </c>
+      <c r="B27" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>501</v>
+      </c>
+      <c r="B33" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>502</v>
+      </c>
+      <c r="B34" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>503</v>
+      </c>
+      <c r="B35" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>504</v>
+      </c>
+      <c r="B36" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>292</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>294</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>296</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>455</v>
+      </c>
+      <c r="B43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>301</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>305</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>307</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>292</v>
+      </c>
+      <c r="B48" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>294</v>
+      </c>
+      <c r="B49" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>296</v>
+      </c>
+      <c r="B50" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>298</v>
+      </c>
+      <c r="B51" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B52" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>301</v>
+      </c>
+      <c r="B53" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>303</v>
+      </c>
+      <c r="B54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>305</v>
+      </c>
+      <c r="B55" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>307</v>
+      </c>
+      <c r="B56" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>505</v>
+      </c>
+      <c r="B57" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>506</v>
+      </c>
+      <c r="B58" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B144"/>
   <sheetViews>
@@ -40134,7 +40661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
@@ -40182,27 +40709,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:90" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
       <c r="T1" t="s">
         <v>370</v>
       </c>
@@ -40220,30 +40747,30 @@
       </c>
     </row>
     <row r="2" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="K2" s="8"/>
+      <c r="M2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="P2" s="9" t="s">
+      <c r="N2" s="8"/>
+      <c r="P2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="8"/>
       <c r="S2" t="s">
         <v>11</v>
       </c>
@@ -40397,60 +40924,60 @@
       <c r="S3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9" t="s">
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9" t="s">
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="9"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
       <c r="AL3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AM3" s="9" t="s">
+      <c r="AM3" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="9" t="s">
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AP3" s="9"/>
-      <c r="AQ3" s="9" t="s">
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="AR3" s="9"/>
-      <c r="AS3" s="9"/>
-      <c r="AT3" s="9"/>
-      <c r="AU3" s="9" t="s">
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="AV3" s="9"/>
-      <c r="AW3" s="9"/>
-      <c r="AX3" s="9"/>
-      <c r="AY3" s="9" t="s">
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="AZ3" s="9"/>
-      <c r="BA3" s="9" t="s">
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="BB3" s="9"/>
-      <c r="BC3" s="9" t="s">
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="BD3" s="9"/>
+      <c r="BD3" s="8"/>
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.25">
       <c r="Y4">
@@ -52865,6 +53392,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="AU3:AX3"/>
+    <mergeCell ref="AQ3:AT3"/>
+    <mergeCell ref="AM3:AN3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="AO3:AP3"/>
     <mergeCell ref="A1:S1"/>
@@ -52877,11 +53409,6 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="AU3:AX3"/>
-    <mergeCell ref="AQ3:AT3"/>
-    <mergeCell ref="AM3:AN3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>